<commit_message>
Alles funktioniert, Fehler lag am zusätzlichen ToDoPanel, das noch nicht gelöscht
</commit_message>
<xml_diff>
--- a/group5/src/main/resources/databases/DefaultCONTRACTS.xlsx
+++ b/group5/src/main/resources/databases/DefaultCONTRACTS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>due_date</t>
   </si>
@@ -666,7 +666,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" t="n">
         <v>4.0</v>
@@ -675,7 +675,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>7500.0</v>
+        <v>75.0</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Alles angepasst, i18n wie in maveb2 eingebaut und funktionsfähig
</commit_message>
<xml_diff>
--- a/group5/src/main/resources/databases/DefaultCONTRACTS.xlsx
+++ b/group5/src/main/resources/databases/DefaultCONTRACTS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
   <si>
     <t>due_date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Sandstein</t>
+  </si>
+  <si>
+    <t>Sprengung</t>
   </si>
 </sst>
 </file>
@@ -666,16 +669,16 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="E6" t="n">
         <v>4.0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>75.0</v>
+        <v>750.0</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>

</xml_diff>